<commit_message>
made a few changes
</commit_message>
<xml_diff>
--- a/TonganZhao/PaulShinn/7 and 11pt.xlsx
+++ b/TonganZhao/PaulShinn/7 and 11pt.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2022SpringCodingCamp\TonganZhao\PaulShinn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE527FA-4AED-4348-B71D-31478E877494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B08CAE6-5CCD-4F3F-8D4D-9417E45470DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21225" yWindow="60" windowWidth="18405" windowHeight="15615" activeTab="3" xr2:uid="{C112BFFF-7BBC-4FD0-B0CB-837E18384276}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C112BFFF-7BBC-4FD0-B0CB-837E18384276}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="96-well map" sheetId="1" r:id="rId1"/>
     <sheet name="Janus 11pt" sheetId="2" r:id="rId2"/>
     <sheet name="FX 11pt" sheetId="8" r:id="rId3"/>
     <sheet name="Platemap 11pt" sheetId="3" r:id="rId4"/>
@@ -3066,8 +3066,8 @@
   </sheetPr>
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13057,8 +13057,8 @@
   </sheetPr>
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>